<commit_message>
Add simple GAMS batch file maker and bug fix v4
</commit_message>
<xml_diff>
--- a/Projects/VTA_bus_project/Data_files/CSV_data/Profile_selection/usurdb_selected_items.xlsx
+++ b/Projects/VTA_bus_project/Data_files/CSV_data/Profile_selection/usurdb_selected_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeichman\Documents\gamsdir\projdir\RODeO\Projects\VTA_bus_project\Data_files\CSV_data\Profile_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE713F65-600B-44B5-BF9E-0B805FF8DB3F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B50C69-4E9E-4F12-87E8-6D0BC0C0AFD4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{EB34CB7E-9B17-4834-A1D5-BEF79A57BD51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="661">
   <si>
     <t>5a33088e5457a305325c48a1</t>
   </si>
@@ -2010,6 +2010,27 @@
   </si>
   <si>
     <t>586fd6da5457a39e6e1c9605</t>
+  </si>
+  <si>
+    <t>A-6</t>
+  </si>
+  <si>
+    <t>A-10</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>A-10 TOU</t>
+  </si>
+  <si>
+    <t>E19 Option R</t>
+  </si>
+  <si>
+    <t>E20 Option R</t>
   </si>
 </sst>
 </file>
@@ -2017,7 +2038,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -2050,7 +2071,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2365,15 +2386,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79A68A2-C84D-4D73-B321-4326122C518F}">
-  <dimension ref="A1:SW28"/>
+  <dimension ref="A1:SW36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="517" max="517" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -7345,6 +7368,62 @@
         <v>43084.571134259262</v>
       </c>
     </row>
+    <row r="30" spans="1:517" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="31" spans="1:517" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>540</v>
+      </c>
+      <c r="C31" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="32" spans="1:517" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>561</v>
+      </c>
+      <c r="C32" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>576</v>
+      </c>
+      <c r="C33" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>607</v>
+      </c>
+      <c r="C34" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>627</v>
+      </c>
+      <c r="C35" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>643</v>
+      </c>
+      <c r="C36" t="s">
+        <v>660</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>